<commit_message>
Modificado o arquivo de validação e de treinamento.
Adicionadas as planilhas dos resultados das propostas 1 e 2 que faltavam. Modificada a planilha da proposta 1 de segunda ordem.
</commit_message>
<xml_diff>
--- a/qualificacao/planilhas/identificacao/P1O2.xlsx
+++ b/qualificacao/planilhas/identificacao/P1O2.xlsx
@@ -7,9 +7,9 @@
     <workbookView xWindow="120" yWindow="135" windowWidth="19320" windowHeight="12075" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="N6" sheetId="5" r:id="rId1"/>
-    <sheet name="N8" sheetId="11" r:id="rId2"/>
-    <sheet name="N10" sheetId="12" r:id="rId3"/>
+    <sheet name="N6" sheetId="14" r:id="rId1"/>
+    <sheet name="N8" sheetId="5" r:id="rId2"/>
+    <sheet name="N10" sheetId="13" r:id="rId3"/>
     <sheet name="Melhores" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="21">
   <si>
     <t>Validação 1</t>
   </si>
@@ -69,6 +69,18 @@
   <si>
     <t>Neurônios C. O.</t>
   </si>
+  <si>
+    <t>Menor EMQ L1</t>
+  </si>
+  <si>
+    <t>Menor EMQ L2</t>
+  </si>
+  <si>
+    <t>Endereço</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
 </sst>
 </file>
 
@@ -99,9 +111,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -151,7 +162,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -231,11 +242,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -270,13 +294,30 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -291,8 +332,11 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -593,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:J20"/>
+  <dimension ref="B2:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="H4" activeCellId="2" sqref="C14:D19 C4:D9 H4:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -607,498 +651,577 @@
     <col min="6" max="6" width="1.42578125" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
     <col min="8" max="10" width="14.42578125" customWidth="1"/>
+    <col min="11" max="11" width="1.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10">
+    <row r="2" spans="2:12">
       <c r="B2" s="1"/>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-    </row>
-    <row r="3" spans="2:10">
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+    </row>
+    <row r="3" spans="2:12">
       <c r="B3" s="2"/>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="12" t="s">
         <v>4</v>
       </c>
       <c r="G3" s="2"/>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:10">
+    <row r="4" spans="2:12">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5">
-        <v>1.6941643000000002E-5</v>
-      </c>
-      <c r="D4" s="5">
-        <v>1.9353394E-5</v>
+      <c r="C4" s="14">
+        <v>1.6941642677942401E-5</v>
+      </c>
+      <c r="D4" s="14">
+        <v>1.935339357523929E-5</v>
       </c>
       <c r="E4" s="5">
         <f t="shared" ref="E4:E9" si="0">SUM(C4:D4)</f>
-        <v>3.6295037000000005E-5</v>
+        <v>3.6295036253181694E-5</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="5">
-        <v>1.3795293000000001E-5</v>
-      </c>
-      <c r="I4" s="5">
-        <v>1.0998126E-5</v>
+      <c r="H4" s="14">
+        <v>1.3795292950998852E-5</v>
+      </c>
+      <c r="I4" s="14">
+        <v>1.0998126263399254E-5</v>
       </c>
       <c r="J4" s="5">
         <f>SUM(H4:I4)</f>
-        <v>2.4793419000000001E-5</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10">
+        <v>2.4793419214398104E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="5">
-        <v>6.1342389999999997E-6</v>
-      </c>
-      <c r="D5" s="5">
-        <v>1.3720184000000001E-5</v>
+      <c r="C5" s="14">
+        <v>6.1342387278308792E-6</v>
+      </c>
+      <c r="D5" s="14">
+        <v>1.3720184270372186E-5</v>
       </c>
       <c r="E5" s="5">
         <f t="shared" si="0"/>
-        <v>1.9854423E-5</v>
+        <v>1.9854422998203064E-5</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="5">
-        <v>1.5835693999999998E-5</v>
-      </c>
-      <c r="I5" s="5">
-        <v>2.9375685999999999E-5</v>
+      <c r="H5" s="14">
+        <v>1.5835693647495047E-5</v>
+      </c>
+      <c r="I5" s="14">
+        <v>2.9375685766226553E-5</v>
       </c>
       <c r="J5" s="5">
         <f t="shared" ref="J5:J9" si="1">SUM(H5:I5)</f>
-        <v>4.5211379999999997E-5</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10">
+        <v>4.5211379413721603E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12">
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="5">
-        <v>1.6376110000000001E-6</v>
-      </c>
-      <c r="D6" s="5">
-        <v>1.38655E-5</v>
+      <c r="C6" s="14">
+        <v>1.6376105080655352E-6</v>
+      </c>
+      <c r="D6" s="14">
+        <v>1.3865500181190913E-5</v>
       </c>
       <c r="E6" s="5">
         <f t="shared" si="0"/>
-        <v>1.5503111000000001E-5</v>
+        <v>1.5503110689256447E-5</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="5">
-        <v>1.638589E-6</v>
-      </c>
-      <c r="I6" s="5">
-        <v>1.3189081E-5</v>
+      <c r="H6" s="14">
+        <v>1.6385886344216231E-6</v>
+      </c>
+      <c r="I6" s="14">
+        <v>1.3189081188716078E-5</v>
       </c>
       <c r="J6" s="5">
         <f t="shared" si="1"/>
-        <v>1.482767E-5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10">
+        <v>1.4827669823137701E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12">
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="5">
-        <v>3.8389597999999997E-5</v>
-      </c>
-      <c r="D7" s="13">
-        <v>3.0722807999999999E-5</v>
+      <c r="C7" s="14">
+        <v>3.8389597938363225E-5</v>
+      </c>
+      <c r="D7" s="14">
+        <v>3.0722808198141273E-5</v>
       </c>
       <c r="E7" s="5">
         <f t="shared" si="0"/>
-        <v>6.9112406000000002E-5</v>
+        <v>6.9112406136504498E-5</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="5">
-        <v>1.6738171999999998E-5</v>
-      </c>
-      <c r="I7" s="5">
-        <v>2.5286109999999999E-5</v>
+      <c r="H7" s="14">
+        <v>1.6738172167235012E-5</v>
+      </c>
+      <c r="I7" s="14">
+        <v>2.5286110267059486E-5</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" si="1"/>
-        <v>4.2024282000000001E-5</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10">
+        <v>4.2024282434294501E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12">
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="5">
-        <v>4.2050359999999997E-6</v>
-      </c>
-      <c r="D8" s="5">
-        <v>1.5043744999999999E-5</v>
+      <c r="C8" s="14">
+        <v>4.2050359270859467E-6</v>
+      </c>
+      <c r="D8" s="14">
+        <v>1.5043744869053773E-5</v>
       </c>
       <c r="E8" s="5">
         <f t="shared" si="0"/>
-        <v>1.9248780999999999E-5</v>
+        <v>1.9248780796139721E-5</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="5">
-        <v>3.4452859999999999E-6</v>
-      </c>
-      <c r="I8" s="5">
-        <v>3.2771641999999998E-5</v>
+      <c r="H8" s="14">
+        <v>3.4452863008527603E-6</v>
+      </c>
+      <c r="I8" s="14">
+        <v>3.277164161499938E-5</v>
       </c>
       <c r="J8" s="5">
         <f t="shared" si="1"/>
-        <v>3.6216927999999999E-5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10">
+        <v>3.6216927915852141E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12">
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="5">
-        <v>1.1738608E-5</v>
-      </c>
-      <c r="D9" s="5">
-        <v>5.5404299999999999E-6</v>
+      <c r="C9" s="14">
+        <v>1.1738607707539159E-5</v>
+      </c>
+      <c r="D9" s="14">
+        <v>5.5404298458723771E-6</v>
       </c>
       <c r="E9" s="5">
         <f t="shared" si="0"/>
-        <v>1.7279037999999999E-5</v>
+        <v>1.7279037553411537E-5</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="5">
-        <v>7.6453320000000003E-6</v>
-      </c>
-      <c r="I9" s="5">
-        <v>8.0587499999999997E-6</v>
+      <c r="H9" s="14">
+        <v>7.6453323473300057E-6</v>
+      </c>
+      <c r="I9" s="14">
+        <v>8.0587504657786825E-6</v>
       </c>
       <c r="J9" s="5">
         <f t="shared" si="1"/>
-        <v>1.5704082000000002E-5</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10">
+        <v>1.570408281310869E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12">
       <c r="B10" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="7">
         <f t="shared" ref="C10:E10" si="2">AVERAGE(C4:C9)</f>
-        <v>1.3174455833333332E-5</v>
+        <v>1.3174455581137858E-5</v>
       </c>
       <c r="D10" s="7">
         <f t="shared" si="2"/>
-        <v>1.6374343499999999E-5</v>
+        <v>1.6374343489978302E-5</v>
       </c>
       <c r="E10" s="7">
         <f t="shared" si="2"/>
-        <v>2.9548799333333334E-5</v>
+        <v>2.9548799071116156E-5</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>11</v>
       </c>
       <c r="H10" s="7">
         <f t="shared" ref="H10:J10" si="3">AVERAGE(H4:H9)</f>
-        <v>9.8497276666666667E-6</v>
+        <v>9.8497276747222177E-6</v>
       </c>
       <c r="I10" s="7">
         <f t="shared" si="3"/>
-        <v>1.9946565833333332E-5</v>
+        <v>1.994656592769657E-5</v>
       </c>
       <c r="J10" s="7">
         <f t="shared" si="3"/>
-        <v>2.97962935E-5</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10">
+        <v>2.9796293602418793E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12">
       <c r="B12" s="1"/>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-    </row>
-    <row r="13" spans="2:10">
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+    </row>
+    <row r="13" spans="2:12">
       <c r="B13" s="2"/>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="12" t="s">
         <v>4</v>
       </c>
       <c r="G13" s="2"/>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="J13" s="13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="2:10">
+    <row r="14" spans="2:12">
       <c r="B14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="5">
-        <v>1.5260719999999999E-5</v>
-      </c>
-      <c r="D14" s="5">
-        <v>1.2178253E-5</v>
+      <c r="C14" s="14">
+        <v>1.5260719529399265E-5</v>
+      </c>
+      <c r="D14" s="14">
+        <v>1.2178252728988274E-5</v>
       </c>
       <c r="E14" s="5">
         <f>SUM(C14:D14)</f>
-        <v>2.7438972999999999E-5</v>
+        <v>2.7438972258387539E-5</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H14" s="5">
-        <f>AVERAGE(C4,H4,C14)</f>
-        <v>1.5332551999999998E-5</v>
+        <f t="shared" ref="H14:I19" si="4">AVERAGE(C4,H4,C14)</f>
+        <v>1.533255171944684E-5</v>
       </c>
       <c r="I14" s="5">
-        <f>AVERAGE(D4,I4,D14)</f>
-        <v>1.4176590999999999E-5</v>
+        <f t="shared" si="4"/>
+        <v>1.4176590855875605E-5</v>
       </c>
       <c r="J14" s="5">
-        <f t="shared" ref="J14:J19" si="4">SUM(H14:I14)</f>
-        <v>2.9509142999999996E-5</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10">
+        <f t="shared" ref="J14:J19" si="5">SUM(H14:I14)</f>
+        <v>2.9509142575322443E-5</v>
+      </c>
+      <c r="L14" s="19" t="str">
+        <f ca="1">IF(J14=MIN($J$14:$J$19),CELL("lin",J14),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="2:12">
       <c r="B15" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="5">
-        <v>2.7162809000000002E-5</v>
-      </c>
-      <c r="D15" s="5">
-        <v>4.1620126000000003E-5</v>
+      <c r="C15" s="14">
+        <v>2.7162808825205686E-5</v>
+      </c>
+      <c r="D15" s="14">
+        <v>4.1620126404561932E-5</v>
       </c>
       <c r="E15" s="5">
-        <f t="shared" ref="E15:E19" si="5">SUM(C15:D15)</f>
-        <v>6.8782935000000011E-5</v>
+        <f t="shared" ref="E15:E19" si="6">SUM(C15:D15)</f>
+        <v>6.8782935229767618E-5</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H15" s="5">
-        <f>AVERAGE(C5,H5,C15)</f>
-        <v>1.6377580666666665E-5</v>
+        <f t="shared" si="4"/>
+        <v>1.6377580400177205E-5</v>
       </c>
       <c r="I15" s="5">
-        <f>AVERAGE(D5,I5,D15)</f>
-        <v>2.8238665333333332E-5</v>
+        <f t="shared" si="4"/>
+        <v>2.8238665480386888E-5</v>
       </c>
       <c r="J15" s="5">
-        <f t="shared" si="4"/>
-        <v>4.4616246000000001E-5</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10">
+        <f t="shared" si="5"/>
+        <v>4.4616245880564093E-5</v>
+      </c>
+      <c r="L15" s="19" t="str">
+        <f t="shared" ref="L15:L19" ca="1" si="7">IF(J15=MIN($J$14:$J$19),CELL("lin",J15),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="2:12">
       <c r="B16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="5">
-        <v>2.099932E-6</v>
-      </c>
-      <c r="D16" s="5">
-        <v>1.2887516E-5</v>
+      <c r="C16" s="14">
+        <v>2.0999324030112053E-6</v>
+      </c>
+      <c r="D16" s="14">
+        <v>1.2887516451968749E-5</v>
       </c>
       <c r="E16" s="5">
-        <f t="shared" si="5"/>
-        <v>1.4987447999999999E-5</v>
+        <f t="shared" si="6"/>
+        <v>1.4987448854979956E-5</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>7</v>
       </c>
       <c r="H16" s="5">
-        <f>AVERAGE(C6,H6,C16)</f>
-        <v>1.7920440000000001E-6</v>
+        <f t="shared" si="4"/>
+        <v>1.7920438484994544E-6</v>
       </c>
       <c r="I16" s="5">
-        <f>AVERAGE(D6,I6,D16)</f>
-        <v>1.3314032333333332E-5</v>
+        <f t="shared" si="4"/>
+        <v>1.3314032607291914E-5</v>
       </c>
       <c r="J16" s="5">
-        <f t="shared" si="4"/>
-        <v>1.5106076333333332E-5</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10">
+        <f t="shared" si="5"/>
+        <v>1.5106076455791368E-5</v>
+      </c>
+      <c r="L16" s="19">
+        <f t="shared" ca="1" si="7"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12">
       <c r="B17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="5">
-        <v>2.5016337000000001E-5</v>
-      </c>
-      <c r="D17" s="5">
-        <v>1.4475722E-5</v>
+      <c r="C17" s="14">
+        <v>2.5016337086856237E-5</v>
+      </c>
+      <c r="D17" s="14">
+        <v>1.4475721681742557E-5</v>
       </c>
       <c r="E17" s="5">
-        <f t="shared" si="5"/>
-        <v>3.9492059000000002E-5</v>
+        <f t="shared" si="6"/>
+        <v>3.9492058768598793E-5</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H17" s="5">
-        <f>AVERAGE(C7,H7,C17)</f>
-        <v>2.6714702333333329E-5</v>
+        <f t="shared" si="4"/>
+        <v>2.6714702397484823E-5</v>
       </c>
       <c r="I17" s="5">
-        <f>AVERAGE(D7,I7,D17)</f>
-        <v>2.349488E-5</v>
+        <f t="shared" si="4"/>
+        <v>2.3494880048981106E-5</v>
       </c>
       <c r="J17" s="5">
-        <f t="shared" si="4"/>
-        <v>5.0209582333333328E-5</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10">
+        <f t="shared" si="5"/>
+        <v>5.0209582446465929E-5</v>
+      </c>
+      <c r="L17" s="19" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="2:12">
       <c r="B18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="5">
-        <v>4.0052150000000004E-6</v>
-      </c>
-      <c r="D18" s="5">
-        <v>1.149262E-5</v>
+      <c r="C18" s="14">
+        <v>4.0052152836954563E-6</v>
+      </c>
+      <c r="D18" s="14">
+        <v>1.1492619859533843E-5</v>
       </c>
       <c r="E18" s="5">
-        <f t="shared" si="5"/>
-        <v>1.5497835000000002E-5</v>
+        <f t="shared" si="6"/>
+        <v>1.5497835143229299E-5</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H18" s="5">
-        <f>AVERAGE(C8,H8,C18)</f>
-        <v>3.8851790000000006E-6</v>
+        <f t="shared" si="4"/>
+        <v>3.8851791705447211E-6</v>
       </c>
       <c r="I18" s="5">
-        <f>AVERAGE(D8,I8,D18)</f>
-        <v>1.9769335666666666E-5</v>
+        <f t="shared" si="4"/>
+        <v>1.9769335447862331E-5</v>
       </c>
       <c r="J18" s="5">
-        <f t="shared" si="4"/>
-        <v>2.3654514666666666E-5</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10">
+        <f t="shared" si="5"/>
+        <v>2.3654514618407052E-5</v>
+      </c>
+      <c r="L18" s="19" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="2:12">
       <c r="B19" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="5">
-        <v>9.1486390000000008E-6</v>
-      </c>
-      <c r="D19" s="5">
-        <v>7.8885999999999993E-6</v>
+      <c r="C19" s="14">
+        <v>9.1486388561120085E-6</v>
+      </c>
+      <c r="D19" s="14">
+        <v>7.8886002956406661E-6</v>
       </c>
       <c r="E19" s="5">
-        <f t="shared" si="5"/>
-        <v>1.7037239E-5</v>
+        <f t="shared" si="6"/>
+        <v>1.7037239151752675E-5</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H19" s="5">
-        <f>AVERAGE(C9,H9,C19)</f>
-        <v>9.5108596666666665E-6</v>
+        <f t="shared" si="4"/>
+        <v>9.5108596369937251E-6</v>
       </c>
       <c r="I19" s="5">
-        <f>AVERAGE(D9,I9,D19)</f>
-        <v>7.162593333333333E-6</v>
+        <f t="shared" si="4"/>
+        <v>7.1625935357639091E-6</v>
       </c>
       <c r="J19" s="5">
-        <f t="shared" si="4"/>
-        <v>1.6673453E-5</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10">
+        <f t="shared" si="5"/>
+        <v>1.6673453172757635E-5</v>
+      </c>
+      <c r="L19" s="19" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="2:12">
       <c r="B20" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="7">
-        <f t="shared" ref="C20:E20" si="6">AVERAGE(C14:C19)</f>
-        <v>1.3782275333333332E-5</v>
+        <f t="shared" ref="C20:E20" si="8">AVERAGE(C14:C19)</f>
+        <v>1.378227533071331E-5</v>
       </c>
       <c r="D20" s="7">
-        <f t="shared" si="6"/>
-        <v>1.6757139500000004E-5</v>
+        <f t="shared" si="8"/>
+        <v>1.6757139570406003E-5</v>
       </c>
       <c r="E20" s="7">
-        <f t="shared" si="6"/>
-        <v>3.0539414833333341E-5</v>
+        <f t="shared" si="8"/>
+        <v>3.0539414901119314E-5</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H20" s="10">
         <f>AVERAGE(H14:H19)</f>
-        <v>1.2268819611111109E-5</v>
+        <v>1.2268819528857798E-5</v>
       </c>
       <c r="I20" s="10">
         <f>AVERAGE(I14:I19)</f>
-        <v>1.7692682944444445E-5</v>
+        <v>1.7692682996026959E-5</v>
       </c>
       <c r="J20" s="10">
         <f>AVERAGE(J14:J19)</f>
-        <v>2.9961502555555554E-5</v>
+        <v>2.9961502524884752E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12">
+      <c r="B21" s="15"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+    </row>
+    <row r="22" spans="2:12">
+      <c r="H22" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12">
+      <c r="G23" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" s="26">
+        <f ca="1">SUM(L14:L19)-13</f>
+        <v>3</v>
+      </c>
+      <c r="I23" s="14" t="str">
+        <f ca="1">CONCATENATE("$H$",SUM(L14:L19))</f>
+        <v>$H$16</v>
+      </c>
+      <c r="J23" s="14">
+        <f ca="1">INDIRECT(I23)</f>
+        <v>1.7920438484994544E-6</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12">
+      <c r="G24" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="27"/>
+      <c r="I24" s="14" t="str">
+        <f ca="1">CONCATENATE("$I$",SUM(L14:L20))</f>
+        <v>$I$16</v>
+      </c>
+      <c r="J24" s="14">
+        <f ca="1">INDIRECT(I24)</f>
+        <v>1.3314032607291914E-5</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="H12:J12"/>
+    <mergeCell ref="H23:H24"/>
   </mergeCells>
   <conditionalFormatting sqref="J14:J19">
     <cfRule type="colorScale" priority="1">
@@ -1119,10 +1242,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:J20"/>
+  <dimension ref="B2:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="I24:J25"/>
+      <selection activeCell="H4" activeCellId="2" sqref="C14:D19 C4:D9 H4:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1133,498 +1256,577 @@
     <col min="6" max="6" width="1.42578125" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
     <col min="8" max="10" width="14.42578125" customWidth="1"/>
+    <col min="11" max="11" width="1.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10">
+    <row r="2" spans="2:12">
       <c r="B2" s="1"/>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-    </row>
-    <row r="3" spans="2:10">
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+    </row>
+    <row r="3" spans="2:12">
       <c r="B3" s="2"/>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G3" s="2"/>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:10">
+    <row r="4" spans="2:12">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5">
-        <v>1.6104447E-5</v>
-      </c>
-      <c r="D4" s="5">
-        <v>3.414167E-6</v>
+      <c r="C4" s="14">
+        <v>1.6104447379736623E-5</v>
+      </c>
+      <c r="D4" s="14">
+        <v>3.4141672333263206E-6</v>
       </c>
       <c r="E4" s="5">
-        <f>SUM(C4:D4)</f>
-        <v>1.9518613999999998E-5</v>
+        <f t="shared" ref="E4:E9" si="0">SUM(C4:D4)</f>
+        <v>1.9518614613062943E-5</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="5">
-        <v>4.4967270000000002E-6</v>
-      </c>
-      <c r="I4" s="5">
-        <v>5.854866E-6</v>
+      <c r="H4" s="14">
+        <v>4.4967272656254845E-6</v>
+      </c>
+      <c r="I4" s="14">
+        <v>5.8548660747602536E-6</v>
       </c>
       <c r="J4" s="5">
         <f>SUM(H4:I4)</f>
-        <v>1.0351593E-5</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10">
+        <v>1.0351593340385738E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="5">
-        <v>4.7846500000000004E-7</v>
-      </c>
-      <c r="D5" s="5">
-        <v>6.55126E-6</v>
+      <c r="C5" s="14">
+        <v>4.7846514480780212E-7</v>
+      </c>
+      <c r="D5" s="14">
+        <v>6.5512597901533048E-6</v>
       </c>
       <c r="E5" s="5">
-        <f t="shared" ref="E5:E9" si="0">SUM(C5:D5)</f>
-        <v>7.0297249999999999E-6</v>
+        <f t="shared" si="0"/>
+        <v>7.0297249349611069E-6</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="5">
-        <v>3.7187600000000001E-7</v>
-      </c>
-      <c r="I5" s="5">
-        <v>2.1942070000000001E-6</v>
+      <c r="H5" s="14">
+        <v>3.7187624755883841E-7</v>
+      </c>
+      <c r="I5" s="14">
+        <v>2.1942066379930597E-6</v>
       </c>
       <c r="J5" s="5">
         <f t="shared" ref="J5:J9" si="1">SUM(H5:I5)</f>
-        <v>2.566083E-6</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10">
+        <v>2.5660828855518982E-6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12">
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="5">
-        <v>8.7051280000000007E-6</v>
-      </c>
-      <c r="D6" s="5">
-        <v>1.5956947000000002E-5</v>
+      <c r="C6" s="14">
+        <v>8.7051275781964326E-6</v>
+      </c>
+      <c r="D6" s="14">
+        <v>1.5956947267721597E-5</v>
       </c>
       <c r="E6" s="5">
         <f t="shared" si="0"/>
-        <v>2.4662075000000001E-5</v>
+        <v>2.4662074845918029E-5</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="5">
-        <v>1.1877089E-5</v>
-      </c>
-      <c r="I6" s="5">
-        <v>1.4174465E-5</v>
+      <c r="H6" s="14">
+        <v>1.1877088963154589E-5</v>
+      </c>
+      <c r="I6" s="14">
+        <v>1.4174465294720935E-5</v>
       </c>
       <c r="J6" s="5">
         <f t="shared" si="1"/>
-        <v>2.6051554000000001E-5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10">
+        <v>2.6051554257875522E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12">
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="5">
-        <v>6.3016190000000003E-6</v>
-      </c>
-      <c r="D7" s="13">
-        <v>9.4532199999999993E-6</v>
+      <c r="C7" s="14">
+        <v>6.3016190733888449E-6</v>
+      </c>
+      <c r="D7" s="14">
+        <v>9.4532203704616427E-6</v>
       </c>
       <c r="E7" s="5">
         <f t="shared" si="0"/>
-        <v>1.5754839E-5</v>
+        <v>1.5754839443850489E-5</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="5">
-        <v>5.2466220000000001E-6</v>
-      </c>
-      <c r="I7" s="5">
-        <v>4.9603910000000004E-6</v>
+      <c r="H7" s="14">
+        <v>5.2466218188779929E-6</v>
+      </c>
+      <c r="I7" s="14">
+        <v>4.9603914170725065E-6</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" si="1"/>
-        <v>1.0207013000000001E-5</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10">
+        <v>1.0207013235950499E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12">
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="5">
-        <v>9.0520010000000001E-6</v>
-      </c>
-      <c r="D8" s="5">
-        <v>1.2440648E-5</v>
+      <c r="C8" s="14">
+        <v>9.0520009172745358E-6</v>
+      </c>
+      <c r="D8" s="14">
+        <v>1.2440648263929578E-5</v>
       </c>
       <c r="E8" s="5">
         <f t="shared" si="0"/>
-        <v>2.1492648999999999E-5</v>
+        <v>2.1492649181204114E-5</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="5">
-        <v>4.1421149999999999E-6</v>
-      </c>
-      <c r="I8" s="5">
-        <v>2.4045376E-5</v>
+      <c r="H8" s="14">
+        <v>4.1421147536811197E-6</v>
+      </c>
+      <c r="I8" s="14">
+        <v>2.4045376469282199E-5</v>
       </c>
       <c r="J8" s="5">
         <f t="shared" si="1"/>
-        <v>2.8187490999999999E-5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10">
+        <v>2.818749122296332E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12">
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="5">
-        <v>3.9052469999999997E-6</v>
-      </c>
-      <c r="D9" s="5">
-        <v>1.9620890000000001E-6</v>
+      <c r="C9" s="14">
+        <v>3.9052469638758851E-6</v>
+      </c>
+      <c r="D9" s="14">
+        <v>1.9620888098864308E-6</v>
       </c>
       <c r="E9" s="5">
         <f t="shared" si="0"/>
-        <v>5.8673359999999999E-6</v>
+        <v>5.8673357737623159E-6</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="5">
-        <v>3.0814170000000001E-6</v>
-      </c>
-      <c r="I9" s="5">
-        <v>3.4824380000000001E-6</v>
+      <c r="H9" s="14">
+        <v>3.0814168080875398E-6</v>
+      </c>
+      <c r="I9" s="14">
+        <v>3.4824375815715844E-6</v>
       </c>
       <c r="J9" s="5">
         <f t="shared" si="1"/>
-        <v>6.5638550000000002E-6</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10">
+        <v>6.5638543896591242E-6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12">
       <c r="B10" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="7">
         <f t="shared" ref="C10:E10" si="2">AVERAGE(C4:C9)</f>
-        <v>7.4244844999999999E-6</v>
+        <v>7.424484509546688E-6</v>
       </c>
       <c r="D10" s="7">
         <f t="shared" si="2"/>
-        <v>8.2963885000000009E-6</v>
+        <v>8.2963886225798139E-6</v>
       </c>
       <c r="E10" s="7">
         <f t="shared" si="2"/>
-        <v>1.5720873E-5</v>
+        <v>1.5720873132126501E-5</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>11</v>
       </c>
       <c r="H10" s="7">
         <f t="shared" ref="H10:J10" si="3">AVERAGE(H4:H9)</f>
-        <v>4.8693076666666672E-6</v>
+        <v>4.8693076428309271E-6</v>
       </c>
       <c r="I10" s="7">
         <f t="shared" si="3"/>
-        <v>9.1186238333333335E-6</v>
+        <v>9.1186239125667554E-6</v>
       </c>
       <c r="J10" s="7">
         <f t="shared" si="3"/>
-        <v>1.39879315E-5</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10">
+        <v>1.3987931555397686E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12">
       <c r="B12" s="1"/>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-    </row>
-    <row r="13" spans="2:10">
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+    </row>
+    <row r="13" spans="2:12">
       <c r="B13" s="2"/>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G13" s="2"/>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="I13" s="12" t="s">
+      <c r="I13" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="J13" s="12" t="s">
+      <c r="J13" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="2:10">
+    <row r="14" spans="2:12">
       <c r="B14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="5">
-        <v>3.2260076000000001E-5</v>
-      </c>
-      <c r="D14" s="5">
-        <v>1.567185E-6</v>
+      <c r="C14" s="14">
+        <v>3.2260076467316277E-5</v>
+      </c>
+      <c r="D14" s="14">
+        <v>1.5671846203443396E-6</v>
       </c>
       <c r="E14" s="5">
         <f>SUM(C14:D14)</f>
-        <v>3.3827261000000001E-5</v>
+        <v>3.3827261087660619E-5</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H14" s="5">
-        <f>AVERAGE(C4,H4,C14)</f>
-        <v>1.7620416666666665E-5</v>
+        <f t="shared" ref="H14:I19" si="4">AVERAGE(C4,H4,C14)</f>
+        <v>1.7620417037559462E-5</v>
       </c>
       <c r="I14" s="5">
-        <f>AVERAGE(D4,I4,D14)</f>
-        <v>3.6120726666666664E-6</v>
+        <f t="shared" si="4"/>
+        <v>3.6120726428103041E-6</v>
       </c>
       <c r="J14" s="5">
-        <f t="shared" ref="J14:J19" si="4">SUM(H14:I14)</f>
-        <v>2.123248933333333E-5</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10">
+        <f t="shared" ref="J14:J19" si="5">SUM(H14:I14)</f>
+        <v>2.1232489680369766E-5</v>
+      </c>
+      <c r="L14" s="19" t="str">
+        <f ca="1">IF(J14=MIN($J$14:$J$19),CELL("lin",J14),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="2:12">
       <c r="B15" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="5">
-        <v>4.66546E-7</v>
-      </c>
-      <c r="D15" s="5">
-        <v>1.128129E-6</v>
+      <c r="C15" s="14">
+        <v>4.6654587051504014E-7</v>
+      </c>
+      <c r="D15" s="14">
+        <v>1.1281292943447041E-6</v>
       </c>
       <c r="E15" s="5">
-        <f t="shared" ref="E15:E19" si="5">SUM(C15:D15)</f>
-        <v>1.5946750000000001E-6</v>
+        <f t="shared" ref="E15:E19" si="6">SUM(C15:D15)</f>
+        <v>1.5946751648597442E-6</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H15" s="5">
-        <f>AVERAGE(C5,H5,C15)</f>
-        <v>4.389623333333333E-7</v>
+        <f t="shared" si="4"/>
+        <v>4.3896242096056019E-7</v>
       </c>
       <c r="I15" s="5">
-        <f>AVERAGE(D5,I5,D15)</f>
-        <v>3.2911986666666661E-6</v>
+        <f t="shared" si="4"/>
+        <v>3.2911985741636896E-6</v>
       </c>
       <c r="J15" s="5">
-        <f t="shared" si="4"/>
-        <v>3.7301609999999994E-6</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10">
+        <f t="shared" si="5"/>
+        <v>3.7301609951242499E-6</v>
+      </c>
+      <c r="L15" s="19">
+        <f t="shared" ref="L15:L19" ca="1" si="7">IF(J15=MIN($J$14:$J$19),CELL("lin",J15),"")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12">
       <c r="B16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="5">
-        <v>1.2659173E-5</v>
-      </c>
-      <c r="D16" s="5">
-        <v>7.6244469999999996E-6</v>
+      <c r="C16" s="14">
+        <v>1.2659173032225965E-5</v>
+      </c>
+      <c r="D16" s="14">
+        <v>7.6244465866144949E-6</v>
       </c>
       <c r="E16" s="5">
-        <f t="shared" si="5"/>
-        <v>2.0283619999999998E-5</v>
+        <f t="shared" si="6"/>
+        <v>2.0283619618840461E-5</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>7</v>
       </c>
       <c r="H16" s="5">
-        <f>AVERAGE(C6,H6,C16)</f>
-        <v>1.1080463333333334E-5</v>
+        <f t="shared" si="4"/>
+        <v>1.1080463191192328E-5</v>
       </c>
       <c r="I16" s="5">
-        <f>AVERAGE(D6,I6,D16)</f>
-        <v>1.2585286333333334E-5</v>
+        <f t="shared" si="4"/>
+        <v>1.2585286383019008E-5</v>
       </c>
       <c r="J16" s="5">
-        <f t="shared" si="4"/>
-        <v>2.3665749666666666E-5</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10">
+        <f t="shared" si="5"/>
+        <v>2.3665749574211336E-5</v>
+      </c>
+      <c r="L16" s="19" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="2:12">
       <c r="B17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="5">
-        <v>4.6850110000000001E-6</v>
-      </c>
-      <c r="D17" s="5">
-        <v>2.9791279999999999E-6</v>
+      <c r="C17" s="14">
+        <v>4.6850112342478358E-6</v>
+      </c>
+      <c r="D17" s="14">
+        <v>2.9791283569272588E-6</v>
       </c>
       <c r="E17" s="5">
-        <f t="shared" si="5"/>
-        <v>7.664139E-6</v>
+        <f t="shared" si="6"/>
+        <v>7.6641395911750954E-6</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H17" s="5">
-        <f>AVERAGE(C7,H7,C17)</f>
-        <v>5.4110840000000001E-6</v>
+        <f t="shared" si="4"/>
+        <v>5.4110840421715573E-6</v>
       </c>
       <c r="I17" s="5">
-        <f>AVERAGE(D7,I7,D17)</f>
-        <v>5.7975796666666665E-6</v>
+        <f t="shared" si="4"/>
+        <v>5.7975800481538024E-6</v>
       </c>
       <c r="J17" s="5">
-        <f t="shared" si="4"/>
-        <v>1.1208663666666667E-5</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10">
+        <f t="shared" si="5"/>
+        <v>1.1208664090325359E-5</v>
+      </c>
+      <c r="L17" s="19" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="2:12">
       <c r="B18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="5">
-        <v>9.6340600000000004E-6</v>
-      </c>
-      <c r="D18" s="5">
-        <v>1.031018E-5</v>
+      <c r="C18" s="14">
+        <v>9.6340598966223634E-6</v>
+      </c>
+      <c r="D18" s="14">
+        <v>1.0310180176217341E-5</v>
       </c>
       <c r="E18" s="5">
-        <f t="shared" si="5"/>
-        <v>1.9944240000000001E-5</v>
+        <f t="shared" si="6"/>
+        <v>1.9944240072839704E-5</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H18" s="5">
-        <f>AVERAGE(C8,H8,C18)</f>
-        <v>7.6093920000000001E-6</v>
+        <f t="shared" si="4"/>
+        <v>7.6093918558593396E-6</v>
       </c>
       <c r="I18" s="5">
-        <f>AVERAGE(D8,I8,D18)</f>
-        <v>1.5598734666666666E-5</v>
+        <f t="shared" si="4"/>
+        <v>1.5598734969809709E-5</v>
       </c>
       <c r="J18" s="5">
-        <f t="shared" si="4"/>
-        <v>2.3208126666666666E-5</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10">
+        <f t="shared" si="5"/>
+        <v>2.3208126825669048E-5</v>
+      </c>
+      <c r="L18" s="19" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="2:12">
       <c r="B19" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="5">
-        <v>4.1129850000000001E-6</v>
-      </c>
-      <c r="D19" s="5">
-        <v>3.240724E-6</v>
+      <c r="C19" s="14">
+        <v>4.1129845373332723E-6</v>
+      </c>
+      <c r="D19" s="14">
+        <v>3.2407244482157866E-6</v>
       </c>
       <c r="E19" s="5">
-        <f t="shared" si="5"/>
-        <v>7.353709E-6</v>
+        <f t="shared" si="6"/>
+        <v>7.3537089855490589E-6</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H19" s="5">
-        <f>AVERAGE(C9,H9,C19)</f>
-        <v>3.6998830000000001E-6</v>
+        <f t="shared" si="4"/>
+        <v>3.6998827697655657E-6</v>
       </c>
       <c r="I19" s="5">
-        <f>AVERAGE(D9,I9,D19)</f>
-        <v>2.8950836666666669E-6</v>
+        <f t="shared" si="4"/>
+        <v>2.8950836132246007E-6</v>
       </c>
       <c r="J19" s="5">
-        <f t="shared" si="4"/>
-        <v>6.594966666666667E-6</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10">
+        <f t="shared" si="5"/>
+        <v>6.594966382990166E-6</v>
+      </c>
+      <c r="L19" s="19" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="2:12">
       <c r="B20" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="7">
-        <f t="shared" ref="C20:E20" si="6">AVERAGE(C14:C19)</f>
-        <v>1.06363085E-5</v>
+        <f t="shared" ref="C20:E20" si="8">AVERAGE(C14:C19)</f>
+        <v>1.0636308506376793E-5</v>
       </c>
       <c r="D20" s="7">
-        <f t="shared" si="6"/>
-        <v>4.4749655000000001E-6</v>
+        <f t="shared" si="8"/>
+        <v>4.474965580443988E-6</v>
       </c>
       <c r="E20" s="7">
-        <f t="shared" si="6"/>
-        <v>1.5111273999999999E-5</v>
+        <f t="shared" si="8"/>
+        <v>1.5111274086820782E-5</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H20" s="10">
         <f>AVERAGE(H14:H19)</f>
-        <v>7.6433668888888896E-6</v>
+        <v>7.6433668862514679E-6</v>
       </c>
       <c r="I20" s="10">
         <f>AVERAGE(I14:I19)</f>
-        <v>7.2966592777777765E-6</v>
+        <v>7.2966593718635188E-6</v>
       </c>
       <c r="J20" s="10">
         <f>AVERAGE(J14:J19)</f>
-        <v>1.4940026166666664E-5</v>
+        <v>1.4940026258114987E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12">
+      <c r="B21" s="15"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+    </row>
+    <row r="22" spans="2:12">
+      <c r="H22" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12">
+      <c r="G23" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" s="26">
+        <f ca="1">SUM(L14:L19)-13</f>
+        <v>2</v>
+      </c>
+      <c r="I23" s="14" t="str">
+        <f ca="1">CONCATENATE("$H$",SUM(L14:L19))</f>
+        <v>$H$15</v>
+      </c>
+      <c r="J23" s="14">
+        <f ca="1">INDIRECT(I23)</f>
+        <v>4.3896242096056019E-7</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12">
+      <c r="G24" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="27"/>
+      <c r="I24" s="14" t="str">
+        <f ca="1">CONCATENATE("$I$",SUM(L14:L20))</f>
+        <v>$I$15</v>
+      </c>
+      <c r="J24" s="14">
+        <f ca="1">INDIRECT(I24)</f>
+        <v>3.2911985741636896E-6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="H12:J12"/>
+    <mergeCell ref="H23:H24"/>
   </mergeCells>
   <conditionalFormatting sqref="J14:J19">
     <cfRule type="colorScale" priority="1">
@@ -1645,10 +1847,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:J20"/>
+  <dimension ref="B2:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18:I18"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1659,498 +1861,577 @@
     <col min="6" max="6" width="1.42578125" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
     <col min="8" max="10" width="14.42578125" customWidth="1"/>
+    <col min="11" max="11" width="1.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10">
+    <row r="2" spans="2:12">
       <c r="B2" s="1"/>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-    </row>
-    <row r="3" spans="2:10">
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+    </row>
+    <row r="3" spans="2:12">
       <c r="B3" s="2"/>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="12" t="s">
         <v>4</v>
       </c>
       <c r="G3" s="2"/>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:10">
+    <row r="4" spans="2:12">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5">
-        <v>9.8233940000000001E-6</v>
-      </c>
-      <c r="D4" s="5">
-        <v>1.1107425999999999E-5</v>
+      <c r="C4" s="14">
+        <v>9.8233938738445901E-6</v>
+      </c>
+      <c r="D4" s="14">
+        <v>1.1107425744356164E-5</v>
       </c>
       <c r="E4" s="5">
-        <f>SUM(C4:D4)</f>
-        <v>2.0930820000000001E-5</v>
+        <f t="shared" ref="E4:E9" si="0">SUM(C4:D4)</f>
+        <v>2.0930819618200754E-5</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="5">
-        <v>1.0077975000000001E-5</v>
-      </c>
-      <c r="I4" s="5">
-        <v>3.2497613000000001E-5</v>
+      <c r="H4" s="14">
+        <v>1.0077974600492818E-5</v>
+      </c>
+      <c r="I4" s="14">
+        <v>3.2497613495578229E-5</v>
       </c>
       <c r="J4" s="5">
         <f>SUM(H4:I4)</f>
-        <v>4.2575588E-5</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10">
+        <v>4.2575588096071046E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="5">
-        <v>6.483497E-6</v>
-      </c>
-      <c r="D5" s="5">
-        <v>1.2607949000000001E-5</v>
+      <c r="C5" s="14">
+        <v>6.4834968783072559E-6</v>
+      </c>
+      <c r="D5" s="14">
+        <v>1.2607949408155129E-5</v>
       </c>
       <c r="E5" s="5">
-        <f t="shared" ref="E5:E9" si="0">SUM(C5:D5)</f>
-        <v>1.9091446000000001E-5</v>
+        <f t="shared" si="0"/>
+        <v>1.9091446286462386E-5</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="5">
-        <v>7.9238030000000001E-6</v>
-      </c>
-      <c r="I5" s="5">
-        <v>3.3073532999999998E-5</v>
+      <c r="H5" s="14">
+        <v>7.9238030605547057E-6</v>
+      </c>
+      <c r="I5" s="14">
+        <v>3.3073533405099827E-5</v>
       </c>
       <c r="J5" s="5">
         <f t="shared" ref="J5:J9" si="1">SUM(H5:I5)</f>
-        <v>4.0997336E-5</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10">
+        <v>4.0997336465654533E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12">
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="5">
-        <v>1.0949254E-5</v>
-      </c>
-      <c r="D6" s="5">
-        <v>6.2055267000000005E-5</v>
+      <c r="C6" s="14">
+        <v>1.094925411111731E-5</v>
+      </c>
+      <c r="D6" s="14">
+        <v>6.2055266858169624E-5</v>
       </c>
       <c r="E6" s="5">
         <f t="shared" si="0"/>
-        <v>7.3004521E-5</v>
+        <v>7.3004520969286937E-5</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="5">
-        <v>1.5253167E-5</v>
-      </c>
-      <c r="I6" s="5">
-        <v>6.6168114999999995E-5</v>
+      <c r="H6" s="14">
+        <v>1.5253166587461339E-5</v>
+      </c>
+      <c r="I6" s="14">
+        <v>6.6168114675829292E-5</v>
       </c>
       <c r="J6" s="5">
         <f t="shared" si="1"/>
-        <v>8.142128199999999E-5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10">
+        <v>8.1421281263290631E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12">
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="5">
-        <v>2.9246920000000001E-5</v>
-      </c>
-      <c r="D7" s="13">
-        <v>1.1610084E-5</v>
+      <c r="C7" s="14">
+        <v>2.924692033627638E-5</v>
+      </c>
+      <c r="D7" s="14">
+        <v>1.1610083641677251E-5</v>
       </c>
       <c r="E7" s="5">
         <f t="shared" si="0"/>
-        <v>4.0857004000000003E-5</v>
+        <v>4.0857003977953633E-5</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="5">
-        <v>1.3513608000000001E-5</v>
-      </c>
-      <c r="I7" s="5">
-        <v>3.0978249999999998E-5</v>
+      <c r="H7" s="14">
+        <v>1.3513607894653939E-5</v>
+      </c>
+      <c r="I7" s="14">
+        <v>3.0978249592675907E-5</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" si="1"/>
-        <v>4.4491857999999998E-5</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10">
+        <v>4.4491857487329844E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12">
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="5">
-        <v>3.978135E-6</v>
-      </c>
-      <c r="D8" s="5">
-        <v>1.3125316E-5</v>
+      <c r="C8" s="14">
+        <v>3.9781345506157695E-6</v>
+      </c>
+      <c r="D8" s="14">
+        <v>1.312531592698646E-5</v>
       </c>
       <c r="E8" s="5">
         <f t="shared" si="0"/>
-        <v>1.7103450999999999E-5</v>
+        <v>1.7103450477602231E-5</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="5">
-        <v>3.1306059999999999E-6</v>
-      </c>
-      <c r="I8" s="5">
-        <v>1.5051957999999999E-5</v>
+      <c r="H8" s="14">
+        <v>3.1306055352892791E-6</v>
+      </c>
+      <c r="I8" s="14">
+        <v>1.505195824236466E-5</v>
       </c>
       <c r="J8" s="5">
         <f t="shared" si="1"/>
-        <v>1.8182563999999999E-5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10">
+        <v>1.8182563777653939E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12">
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="5">
-        <v>7.7840810000000003E-6</v>
-      </c>
-      <c r="D9" s="5">
-        <v>1.5162074000000001E-5</v>
+      <c r="C9" s="14">
+        <v>7.7840813734859579E-6</v>
+      </c>
+      <c r="D9" s="14">
+        <v>1.5162073704115483E-5</v>
       </c>
       <c r="E9" s="5">
         <f t="shared" si="0"/>
-        <v>2.2946155000000001E-5</v>
+        <v>2.2946155077601443E-5</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="5">
-        <v>4.2077079999999998E-6</v>
-      </c>
-      <c r="I9" s="5">
-        <v>4.5579896000000003E-5</v>
+      <c r="H9" s="14">
+        <v>4.2077083999147668E-6</v>
+      </c>
+      <c r="I9" s="14">
+        <v>4.5579895810784559E-5</v>
       </c>
       <c r="J9" s="5">
         <f t="shared" si="1"/>
-        <v>4.9787604000000002E-5</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10">
+        <v>4.9787604210699325E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12">
       <c r="B10" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="7">
         <f t="shared" ref="C10:E10" si="2">AVERAGE(C4:C9)</f>
-        <v>1.1377546833333333E-5</v>
+        <v>1.1377546853941209E-5</v>
       </c>
       <c r="D10" s="7">
         <f t="shared" si="2"/>
-        <v>2.0944686000000001E-5</v>
+        <v>2.0944685880576684E-5</v>
       </c>
       <c r="E10" s="7">
         <f t="shared" si="2"/>
-        <v>3.2322232833333329E-5</v>
+        <v>3.2322232734517903E-5</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>11</v>
       </c>
       <c r="H10" s="7">
         <f t="shared" ref="H10:J10" si="3">AVERAGE(H4:H9)</f>
-        <v>9.017811166666667E-6</v>
+        <v>9.0178110130611417E-6</v>
       </c>
       <c r="I10" s="7">
         <f t="shared" si="3"/>
-        <v>3.7224894166666668E-5</v>
+        <v>3.7224894203722083E-5</v>
       </c>
       <c r="J10" s="7">
         <f t="shared" si="3"/>
-        <v>4.6242705333333327E-5</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10">
+        <v>4.624270521678322E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12">
       <c r="B12" s="1"/>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-    </row>
-    <row r="13" spans="2:10">
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+    </row>
+    <row r="13" spans="2:12">
       <c r="B13" s="2"/>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="12" t="s">
         <v>4</v>
       </c>
       <c r="G13" s="2"/>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="I13" s="12" t="s">
+      <c r="I13" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="J13" s="12" t="s">
+      <c r="J13" s="13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="2:10">
+    <row r="14" spans="2:12">
       <c r="B14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="5">
-        <v>1.1246759999999999E-5</v>
-      </c>
-      <c r="D14" s="5">
-        <v>1.3784165E-5</v>
+      <c r="C14" s="14">
+        <v>1.1246760176501513E-5</v>
+      </c>
+      <c r="D14" s="14">
+        <v>1.3784164546520055E-5</v>
       </c>
       <c r="E14" s="5">
         <f>SUM(C14:D14)</f>
-        <v>2.5030925E-5</v>
+        <v>2.5030924723021567E-5</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H14" s="5">
-        <f>AVERAGE(C4,H4,C14)</f>
-        <v>1.0382709666666667E-5</v>
+        <f t="shared" ref="H14:I19" si="4">AVERAGE(C4,H4,C14)</f>
+        <v>1.0382709550279639E-5</v>
       </c>
       <c r="I14" s="5">
-        <f>AVERAGE(D4,I4,D14)</f>
-        <v>1.9129734666666667E-5</v>
+        <f t="shared" si="4"/>
+        <v>1.9129734595484816E-5</v>
       </c>
       <c r="J14" s="5">
-        <f t="shared" ref="J14:J19" si="4">SUM(H14:I14)</f>
-        <v>2.9512444333333336E-5</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10">
+        <f t="shared" ref="J14:J19" si="5">SUM(H14:I14)</f>
+        <v>2.9512444145764456E-5</v>
+      </c>
+      <c r="L14" s="19" t="str">
+        <f ca="1">IF(J14=MIN($J$14:$J$19),CELL("lin",J14),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="2:12">
       <c r="B15" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="5">
-        <v>6.8121829999999999E-6</v>
-      </c>
-      <c r="D15" s="5">
-        <v>1.1239329E-5</v>
+      <c r="C15" s="14">
+        <v>6.8121831069391784E-6</v>
+      </c>
+      <c r="D15" s="14">
+        <v>1.1239329104458362E-5</v>
       </c>
       <c r="E15" s="5">
-        <f t="shared" ref="E15:E19" si="5">SUM(C15:D15)</f>
-        <v>1.8051512000000001E-5</v>
+        <f t="shared" ref="E15:E19" si="6">SUM(C15:D15)</f>
+        <v>1.8051512211397541E-5</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H15" s="5">
-        <f>AVERAGE(C5,H5,C15)</f>
-        <v>7.0731609999999994E-6</v>
+        <f t="shared" si="4"/>
+        <v>7.0731610152670466E-6</v>
       </c>
       <c r="I15" s="5">
-        <f>AVERAGE(D5,I5,D15)</f>
-        <v>1.8973603666666665E-5</v>
+        <f t="shared" si="4"/>
+        <v>1.8973603972571106E-5</v>
       </c>
       <c r="J15" s="5">
-        <f t="shared" si="4"/>
-        <v>2.6046764666666664E-5</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10">
+        <f t="shared" si="5"/>
+        <v>2.6046764987838152E-5</v>
+      </c>
+      <c r="L15" s="19" t="str">
+        <f t="shared" ref="L15:L19" ca="1" si="7">IF(J15=MIN($J$14:$J$19),CELL("lin",J15),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="2:12">
       <c r="B16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="5">
-        <v>1.4510123E-5</v>
-      </c>
-      <c r="D16" s="5">
-        <v>2.8014263999999999E-5</v>
+      <c r="C16" s="14">
+        <v>1.4510122672661896E-5</v>
+      </c>
+      <c r="D16" s="14">
+        <v>2.8014264201193996E-5</v>
       </c>
       <c r="E16" s="5">
-        <f t="shared" si="5"/>
-        <v>4.2524387E-5</v>
+        <f t="shared" si="6"/>
+        <v>4.2524386873855896E-5</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>7</v>
       </c>
       <c r="H16" s="5">
-        <f>AVERAGE(C6,H6,C16)</f>
-        <v>1.3570848E-5</v>
+        <f t="shared" si="4"/>
+        <v>1.3570847790413515E-5</v>
       </c>
       <c r="I16" s="5">
-        <f>AVERAGE(D6,I6,D16)</f>
-        <v>5.2079215333333339E-5</v>
+        <f t="shared" si="4"/>
+        <v>5.2079215245064299E-5</v>
       </c>
       <c r="J16" s="5">
-        <f t="shared" si="4"/>
-        <v>6.5650063333333339E-5</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10">
+        <f t="shared" si="5"/>
+        <v>6.5650063035477821E-5</v>
+      </c>
+      <c r="L16" s="19" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="2:12">
       <c r="B17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="5">
-        <v>3.3456544000000001E-5</v>
-      </c>
-      <c r="D17" s="5">
-        <v>1.0072765E-5</v>
+      <c r="C17" s="14">
+        <v>3.345654407010778E-5</v>
+      </c>
+      <c r="D17" s="14">
+        <v>1.0072764681526918E-5</v>
       </c>
       <c r="E17" s="5">
-        <f t="shared" si="5"/>
-        <v>4.3529309000000001E-5</v>
+        <f t="shared" si="6"/>
+        <v>4.3529308751634701E-5</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H17" s="5">
-        <f>AVERAGE(C7,H7,C17)</f>
-        <v>2.5405690666666669E-5</v>
+        <f t="shared" si="4"/>
+        <v>2.54056907670127E-5</v>
       </c>
       <c r="I17" s="5">
-        <f>AVERAGE(D7,I7,D17)</f>
-        <v>1.7553699666666668E-5</v>
+        <f t="shared" si="4"/>
+        <v>1.7553699305293359E-5</v>
       </c>
       <c r="J17" s="5">
-        <f t="shared" si="4"/>
-        <v>4.2959390333333337E-5</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10">
+        <f t="shared" si="5"/>
+        <v>4.295939007230606E-5</v>
+      </c>
+      <c r="L17" s="19" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="2:12">
       <c r="B18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="5">
-        <v>3.7171010000000002E-6</v>
-      </c>
-      <c r="D18" s="5">
-        <v>1.3856686000000001E-5</v>
+      <c r="C18" s="14">
+        <v>3.7171014593301386E-6</v>
+      </c>
+      <c r="D18" s="14">
+        <v>1.3856685597410498E-5</v>
       </c>
       <c r="E18" s="5">
-        <f t="shared" si="5"/>
-        <v>1.7573787000000002E-5</v>
+        <f t="shared" si="6"/>
+        <v>1.7573787056740635E-5</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H18" s="5">
-        <f>AVERAGE(C8,H8,C18)</f>
-        <v>3.608614E-6</v>
+        <f t="shared" si="4"/>
+        <v>3.6086138484117291E-6</v>
       </c>
       <c r="I18" s="5">
-        <f>AVERAGE(D8,I8,D18)</f>
-        <v>1.4011320000000001E-5</v>
+        <f t="shared" si="4"/>
+        <v>1.4011319922253874E-5</v>
       </c>
       <c r="J18" s="5">
-        <f t="shared" si="4"/>
-        <v>1.7619934E-5</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10">
+        <f t="shared" si="5"/>
+        <v>1.7619933770665603E-5</v>
+      </c>
+      <c r="L18" s="19">
+        <f t="shared" ca="1" si="7"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12">
       <c r="B19" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="5">
-        <v>6.1566230000000001E-6</v>
-      </c>
-      <c r="D19" s="5">
-        <v>9.9582069999999998E-6</v>
+      <c r="C19" s="14">
+        <v>6.1566229875189823E-6</v>
+      </c>
+      <c r="D19" s="14">
+        <v>9.9582069179624448E-6</v>
       </c>
       <c r="E19" s="5">
-        <f t="shared" si="5"/>
-        <v>1.6114829999999999E-5</v>
+        <f t="shared" si="6"/>
+        <v>1.6114829905481429E-5</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H19" s="5">
-        <f>AVERAGE(C9,H9,C19)</f>
-        <v>6.049470666666667E-6</v>
+        <f t="shared" si="4"/>
+        <v>6.0494709203065681E-6</v>
       </c>
       <c r="I19" s="5">
-        <f>AVERAGE(D9,I9,D19)</f>
-        <v>2.3566725666666671E-5</v>
+        <f t="shared" si="4"/>
+        <v>2.3566725477620829E-5</v>
       </c>
       <c r="J19" s="5">
-        <f t="shared" si="4"/>
-        <v>2.9616196333333338E-5</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10">
+        <f t="shared" si="5"/>
+        <v>2.9616196397927397E-5</v>
+      </c>
+      <c r="L19" s="19" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="2:12">
       <c r="B20" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="7">
-        <f t="shared" ref="C20:E20" si="6">AVERAGE(C14:C19)</f>
-        <v>1.2649888999999999E-5</v>
+        <f t="shared" ref="C20:E20" si="8">AVERAGE(C14:C19)</f>
+        <v>1.2649889078843247E-5</v>
       </c>
       <c r="D20" s="7">
-        <f t="shared" si="6"/>
-        <v>1.4487569333333333E-5</v>
+        <f t="shared" si="8"/>
+        <v>1.4487569174845378E-5</v>
       </c>
       <c r="E20" s="7">
-        <f t="shared" si="6"/>
-        <v>2.7137458333333334E-5</v>
+        <f t="shared" si="8"/>
+        <v>2.7137458253688628E-5</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H20" s="10">
         <f>AVERAGE(H14:H19)</f>
-        <v>1.1015082333333335E-5</v>
+        <v>1.1015082315281866E-5</v>
       </c>
       <c r="I20" s="10">
         <f>AVERAGE(I14:I19)</f>
-        <v>2.4219049833333335E-5</v>
+        <v>2.4219049753048045E-5</v>
       </c>
       <c r="J20" s="10">
         <f>AVERAGE(J14:J19)</f>
-        <v>3.5234132166666671E-5</v>
+        <v>3.5234132068329914E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12">
+      <c r="B21" s="15"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+    </row>
+    <row r="22" spans="2:12">
+      <c r="H22" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12">
+      <c r="G23" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" s="26">
+        <f ca="1">SUM(L14:L19)-13</f>
+        <v>5</v>
+      </c>
+      <c r="I23" s="14" t="str">
+        <f ca="1">CONCATENATE("$H$",SUM(L14:L19))</f>
+        <v>$H$18</v>
+      </c>
+      <c r="J23" s="14">
+        <f ca="1">INDIRECT(I23)</f>
+        <v>3.6086138484117291E-6</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12">
+      <c r="G24" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="27"/>
+      <c r="I24" s="14" t="str">
+        <f ca="1">CONCATENATE("$I$",SUM(L14:L20))</f>
+        <v>$I$18</v>
+      </c>
+      <c r="J24" s="14">
+        <f ca="1">INDIRECT(I24)</f>
+        <v>1.4011319922253874E-5</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="H12:J12"/>
+    <mergeCell ref="H23:H24"/>
   </mergeCells>
   <conditionalFormatting sqref="J14:J19">
     <cfRule type="colorScale" priority="1">
@@ -2165,7 +2446,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2174,7 +2455,7 @@
   <dimension ref="B3:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2187,13 +2468,13 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:6" ht="15" customHeight="1">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="11" t="s">
@@ -2213,63 +2494,66 @@
       </c>
     </row>
     <row r="5" spans="2:6">
-      <c r="B5" s="14">
+      <c r="B5" s="21">
         <v>6</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="14">
+        <f ca="1">'N6'!H23</f>
         <v>3</v>
       </c>
-      <c r="D5" s="19">
-        <f>'N6'!H16</f>
-        <v>1.7920440000000001E-6</v>
-      </c>
-      <c r="E5" s="19">
-        <f>'N6'!I16</f>
-        <v>1.3314032333333332E-5</v>
-      </c>
-      <c r="F5" s="19">
-        <f>'N6'!J16</f>
-        <v>1.5106076333333332E-5</v>
+      <c r="D5" s="14">
+        <f ca="1">'N6'!J23</f>
+        <v>1.7920438484994544E-6</v>
+      </c>
+      <c r="E5" s="14">
+        <f ca="1">'N6'!J24</f>
+        <v>1.3314032607291914E-5</v>
+      </c>
+      <c r="F5" s="14">
+        <f ca="1">SUM(D5:E5)</f>
+        <v>1.5106076455791368E-5</v>
       </c>
     </row>
     <row r="6" spans="2:6">
-      <c r="B6" s="14">
+      <c r="B6" s="21">
         <v>8</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="14">
+        <f ca="1">'N8'!H23</f>
         <v>2</v>
       </c>
-      <c r="D6" s="19">
-        <f>'N8'!H15</f>
-        <v>4.389623333333333E-7</v>
-      </c>
-      <c r="E6" s="19">
-        <f>'N8'!I15</f>
-        <v>3.2911986666666661E-6</v>
-      </c>
-      <c r="F6" s="19">
-        <f>'N8'!J15</f>
-        <v>3.7301609999999994E-6</v>
+      <c r="D6" s="14">
+        <f ca="1">'N8'!J23</f>
+        <v>4.3896242096056019E-7</v>
+      </c>
+      <c r="E6" s="14">
+        <f ca="1">'N8'!J24</f>
+        <v>3.2911985741636896E-6</v>
+      </c>
+      <c r="F6" s="14">
+        <f t="shared" ref="F6:F7" ca="1" si="0">SUM(D6:E6)</f>
+        <v>3.7301609951242499E-6</v>
       </c>
     </row>
     <row r="7" spans="2:6">
-      <c r="B7" s="14">
+      <c r="B7" s="21">
         <v>10</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="14">
+        <f ca="1">'N10'!H23</f>
         <v>5</v>
       </c>
       <c r="D7" s="5">
-        <f>'N10'!H18</f>
-        <v>3.608614E-6</v>
+        <f ca="1">'N10'!J23</f>
+        <v>3.6086138484117291E-6</v>
       </c>
       <c r="E7" s="5">
-        <f>'N10'!I18</f>
-        <v>1.4011320000000001E-5</v>
-      </c>
-      <c r="F7" s="19">
-        <f>'N10'!J18</f>
-        <v>1.7619934E-5</v>
+        <f ca="1">'N10'!J24</f>
+        <v>1.4011319922253874E-5</v>
+      </c>
+      <c r="F7" s="14">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.7619933770665603E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adição de todas as planilhas das redes de identificação.
</commit_message>
<xml_diff>
--- a/qualificacao/planilhas/identificacao/P1O2.xlsx
+++ b/qualificacao/planilhas/identificacao/P1O2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="19320" windowHeight="12075" activeTab="3"/>
@@ -12,12 +12,12 @@
     <sheet name="N10" sheetId="13" r:id="rId3"/>
     <sheet name="Melhores" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="22">
   <si>
     <t>Validação 1</t>
   </si>
@@ -81,12 +81,15 @@
   <si>
     <t>Valor</t>
   </si>
+  <si>
+    <t>Melhor Rede</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,8 +120,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -158,6 +169,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -259,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -337,6 +354,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -427,6 +450,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -461,6 +485,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -636,14 +661,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" activeCellId="2" sqref="C14:D19 C4:D9 H4:I9"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.42578125" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
@@ -654,7 +679,7 @@
     <col min="11" max="11" width="1.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="22" t="s">
         <v>0</v>
@@ -668,7 +693,7 @@
       <c r="I2" s="24"/>
       <c r="J2" s="24"/>
     </row>
-    <row r="3" spans="2:12">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="12" t="s">
         <v>2</v>
@@ -690,7 +715,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:12">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -718,7 +743,7 @@
         <v>2.4793419214398104E-5</v>
       </c>
     </row>
-    <row r="5" spans="2:12">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
@@ -746,7 +771,7 @@
         <v>4.5211379413721603E-5</v>
       </c>
     </row>
-    <row r="6" spans="2:12">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
@@ -774,7 +799,7 @@
         <v>1.4827669823137701E-5</v>
       </c>
     </row>
-    <row r="7" spans="2:12">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
@@ -802,7 +827,7 @@
         <v>4.2024282434294501E-5</v>
       </c>
     </row>
-    <row r="8" spans="2:12">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -830,7 +855,7 @@
         <v>3.6216927915852141E-5</v>
       </c>
     </row>
-    <row r="9" spans="2:12">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
@@ -858,7 +883,7 @@
         <v>1.570408281310869E-5</v>
       </c>
     </row>
-    <row r="10" spans="2:12">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>11</v>
       </c>
@@ -890,7 +915,7 @@
         <v>2.9796293602418793E-5</v>
       </c>
     </row>
-    <row r="12" spans="2:12">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="24" t="s">
         <v>12</v>
@@ -904,7 +929,7 @@
       <c r="I12" s="25"/>
       <c r="J12" s="25"/>
     </row>
-    <row r="13" spans="2:12">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="12" t="s">
         <v>2</v>
@@ -926,7 +951,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="2:12">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>5</v>
       </c>
@@ -960,7 +985,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="2:12">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>6</v>
       </c>
@@ -994,7 +1019,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="2:12">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>7</v>
       </c>
@@ -1028,7 +1053,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="2:12">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>8</v>
       </c>
@@ -1062,7 +1087,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:12">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>9</v>
       </c>
@@ -1096,7 +1121,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="2:12">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>10</v>
       </c>
@@ -1130,7 +1155,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:12">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
         <v>11</v>
       </c>
@@ -1162,7 +1187,7 @@
         <v>2.9961502524884752E-5</v>
       </c>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="15"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
@@ -1173,7 +1198,7 @@
       <c r="I21" s="16"/>
       <c r="J21" s="16"/>
     </row>
-    <row r="22" spans="2:12">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H22" s="20" t="s">
         <v>14</v>
       </c>
@@ -1184,7 +1209,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="2:12">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G23" s="18" t="s">
         <v>17</v>
       </c>
@@ -1201,7 +1226,7 @@
         <v>1.7920438484994544E-6</v>
       </c>
     </row>
-    <row r="24" spans="2:12">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G24" s="18" t="s">
         <v>18</v>
       </c>
@@ -1226,9 +1251,9 @@
   <conditionalFormatting sqref="J14:J19">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -1241,14 +1266,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" activeCellId="2" sqref="C14:D19 C4:D9 H4:I9"/>
+      <selection activeCell="H23" sqref="H23:H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.42578125" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
@@ -1259,7 +1284,7 @@
     <col min="11" max="11" width="1.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="22" t="s">
         <v>0</v>
@@ -1273,7 +1298,7 @@
       <c r="I2" s="24"/>
       <c r="J2" s="24"/>
     </row>
-    <row r="3" spans="2:12">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="3" t="s">
         <v>2</v>
@@ -1295,7 +1320,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:12">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -1323,7 +1348,7 @@
         <v>1.0351593340385738E-5</v>
       </c>
     </row>
-    <row r="5" spans="2:12">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
@@ -1351,7 +1376,7 @@
         <v>2.5660828855518982E-6</v>
       </c>
     </row>
-    <row r="6" spans="2:12">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1379,7 +1404,7 @@
         <v>2.6051554257875522E-5</v>
       </c>
     </row>
-    <row r="7" spans="2:12">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1407,7 +1432,7 @@
         <v>1.0207013235950499E-5</v>
       </c>
     </row>
-    <row r="8" spans="2:12">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1435,7 +1460,7 @@
         <v>2.818749122296332E-5</v>
       </c>
     </row>
-    <row r="9" spans="2:12">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
@@ -1463,7 +1488,7 @@
         <v>6.5638543896591242E-6</v>
       </c>
     </row>
-    <row r="10" spans="2:12">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>11</v>
       </c>
@@ -1495,7 +1520,7 @@
         <v>1.3987931555397686E-5</v>
       </c>
     </row>
-    <row r="12" spans="2:12">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="24" t="s">
         <v>12</v>
@@ -1509,7 +1534,7 @@
       <c r="I12" s="25"/>
       <c r="J12" s="25"/>
     </row>
-    <row r="13" spans="2:12">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="3" t="s">
         <v>2</v>
@@ -1531,7 +1556,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="2:12">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>5</v>
       </c>
@@ -1565,7 +1590,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="2:12">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>6</v>
       </c>
@@ -1599,7 +1624,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="2:12">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>7</v>
       </c>
@@ -1633,7 +1658,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:12">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>8</v>
       </c>
@@ -1667,7 +1692,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:12">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>9</v>
       </c>
@@ -1701,7 +1726,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="2:12">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>10</v>
       </c>
@@ -1735,7 +1760,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:12">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
         <v>11</v>
       </c>
@@ -1767,7 +1792,7 @@
         <v>1.4940026258114987E-5</v>
       </c>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="15"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
@@ -1778,7 +1803,7 @@
       <c r="I21" s="16"/>
       <c r="J21" s="16"/>
     </row>
-    <row r="22" spans="2:12">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H22" s="20" t="s">
         <v>14</v>
       </c>
@@ -1789,7 +1814,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="2:12">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G23" s="18" t="s">
         <v>17</v>
       </c>
@@ -1806,7 +1831,7 @@
         <v>4.3896242096056019E-7</v>
       </c>
     </row>
-    <row r="24" spans="2:12">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G24" s="18" t="s">
         <v>18</v>
       </c>
@@ -1831,9 +1856,9 @@
   <conditionalFormatting sqref="J14:J19">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -1846,14 +1871,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.42578125" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
@@ -1864,7 +1889,7 @@
     <col min="11" max="11" width="1.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="22" t="s">
         <v>0</v>
@@ -1878,7 +1903,7 @@
       <c r="I2" s="24"/>
       <c r="J2" s="24"/>
     </row>
-    <row r="3" spans="2:12">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="12" t="s">
         <v>2</v>
@@ -1900,7 +1925,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:12">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -1928,7 +1953,7 @@
         <v>4.2575588096071046E-5</v>
       </c>
     </row>
-    <row r="5" spans="2:12">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
@@ -1956,7 +1981,7 @@
         <v>4.0997336465654533E-5</v>
       </c>
     </row>
-    <row r="6" spans="2:12">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1984,7 +2009,7 @@
         <v>8.1421281263290631E-5</v>
       </c>
     </row>
-    <row r="7" spans="2:12">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
@@ -2012,7 +2037,7 @@
         <v>4.4491857487329844E-5</v>
       </c>
     </row>
-    <row r="8" spans="2:12">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -2040,7 +2065,7 @@
         <v>1.8182563777653939E-5</v>
       </c>
     </row>
-    <row r="9" spans="2:12">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
@@ -2068,7 +2093,7 @@
         <v>4.9787604210699325E-5</v>
       </c>
     </row>
-    <row r="10" spans="2:12">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>11</v>
       </c>
@@ -2100,7 +2125,7 @@
         <v>4.624270521678322E-5</v>
       </c>
     </row>
-    <row r="12" spans="2:12">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="24" t="s">
         <v>12</v>
@@ -2114,7 +2139,7 @@
       <c r="I12" s="25"/>
       <c r="J12" s="25"/>
     </row>
-    <row r="13" spans="2:12">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="12" t="s">
         <v>2</v>
@@ -2136,7 +2161,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="2:12">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>5</v>
       </c>
@@ -2170,7 +2195,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="2:12">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>6</v>
       </c>
@@ -2204,7 +2229,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="2:12">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>7</v>
       </c>
@@ -2238,7 +2263,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:12">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>8</v>
       </c>
@@ -2272,7 +2297,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:12">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>9</v>
       </c>
@@ -2306,7 +2331,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="2:12">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>10</v>
       </c>
@@ -2340,7 +2365,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:12">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
         <v>11</v>
       </c>
@@ -2372,7 +2397,7 @@
         <v>3.5234132068329914E-5</v>
       </c>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="15"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
@@ -2383,7 +2408,7 @@
       <c r="I21" s="16"/>
       <c r="J21" s="16"/>
     </row>
-    <row r="22" spans="2:12">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H22" s="20" t="s">
         <v>14</v>
       </c>
@@ -2394,7 +2419,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="2:12">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G23" s="18" t="s">
         <v>17</v>
       </c>
@@ -2411,7 +2436,7 @@
         <v>3.6086138484117291E-6</v>
       </c>
     </row>
-    <row r="24" spans="2:12">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G24" s="18" t="s">
         <v>18</v>
       </c>
@@ -2436,9 +2461,9 @@
   <conditionalFormatting sqref="J14:J19">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -2451,14 +2476,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.42578125" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
@@ -2467,7 +2492,7 @@
     <col min="7" max="7" width="1.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" ht="15" customHeight="1">
+    <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="24" t="s">
         <v>15</v>
       </c>
@@ -2476,7 +2501,7 @@
       <c r="E3" s="24"/>
       <c r="F3" s="24"/>
     </row>
-    <row r="4" spans="2:6">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
         <v>16</v>
       </c>
@@ -2493,7 +2518,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="21">
         <v>6</v>
       </c>
@@ -2513,8 +2538,12 @@
         <f ca="1">SUM(D5:E5)</f>
         <v>1.5106076455791368E-5</v>
       </c>
-    </row>
-    <row r="6" spans="2:6">
+      <c r="H5" s="19" t="str">
+        <f ca="1">IF(F5=MIN($F$5:$F$7),CELL("lin",F5),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="21">
         <v>8</v>
       </c>
@@ -2534,8 +2563,12 @@
         <f t="shared" ref="F6:F7" ca="1" si="0">SUM(D6:E6)</f>
         <v>3.7301609951242499E-6</v>
       </c>
-    </row>
-    <row r="7" spans="2:6">
+      <c r="H6" s="19">
+        <f t="shared" ref="H6:H7" ca="1" si="1">IF(F6=MIN($F$5:$F$7),CELL("lin",F6),"")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="21">
         <v>10</v>
       </c>
@@ -2555,17 +2588,70 @@
         <f t="shared" ca="1" si="0"/>
         <v>1.7619933770665603E-5</v>
       </c>
+      <c r="H7" s="19" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="14">
+        <f ca="1">INDIRECT(CONCATENATE("$B$",SUM($H$5:$H$7)))</f>
+        <v>8</v>
+      </c>
+      <c r="C11" s="14">
+        <f ca="1">INDIRECT(CONCATENATE("$C$",SUM($H$5:$H$7)))</f>
+        <v>2</v>
+      </c>
+      <c r="D11" s="14">
+        <f ca="1">INDIRECT(CONCATENATE("$D$",SUM($H$5:$H$7)))</f>
+        <v>4.3896242096056019E-7</v>
+      </c>
+      <c r="E11" s="14">
+        <f ca="1">INDIRECT(CONCATENATE("$E$",SUM($H$5:$H$7)))</f>
+        <v>3.2911985741636896E-6</v>
+      </c>
+      <c r="F11" s="14">
+        <f ca="1">INDIRECT(CONCATENATE("$F$",SUM($H$5:$H$7)))</f>
+        <v>3.7301609951242499E-6</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B9:F9"/>
   </mergeCells>
   <conditionalFormatting sqref="F5:F7">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -2573,5 +2659,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>